<commit_message>
fixed sections seed file
</commit_message>
<xml_diff>
--- a/Sections.xlsx
+++ b/Sections.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Introduction to Astronomy: Crash Course Astronomy #1</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/Yocja_N5s1I?list=PLBDA2E52FB1EF80C9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vid </t>
   </si>
   <si>
     <t>Indus Valley Civilization: Crash Course World History #2</t>
@@ -467,7 +464,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -579,13 +576,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -596,13 +593,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -613,13 +610,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -630,13 +627,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -647,13 +644,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -664,13 +661,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -681,13 +678,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -698,13 +695,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>8</v>
@@ -715,13 +712,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>9</v>
@@ -732,13 +729,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -749,13 +746,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -766,13 +763,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>11</v>
@@ -783,13 +780,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <v>11</v>
@@ -800,13 +797,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <v>11</v>

</xml_diff>